<commit_message>
Implemented Spectrum Range at each location per company
</commit_message>
<xml_diff>
--- a/Excel/spectrumRange.xlsx
+++ b/Excel/spectrumRange.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\IIITD\FIRST_SEM\OOPD\Project\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B760292-9A8B-47BC-8FBB-1B2F50FF71BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E6F406-1903-46C7-AE9C-3C8BCD9C9C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spectrumRange" sheetId="1" r:id="rId1"/>
@@ -548,7 +548,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -654,7 +654,7 @@
         <v>1.038463535506799E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>41122</v>
       </c>
@@ -671,7 +671,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43648</v>
       </c>
@@ -688,7 +688,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>40123</v>
       </c>
@@ -705,7 +705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -722,7 +722,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -739,7 +739,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>24</v>
       </c>
@@ -756,7 +756,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>25</v>
       </c>
@@ -773,7 +773,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>39638</v>
       </c>
@@ -790,7 +790,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>26</v>
       </c>
@@ -807,7 +807,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -824,7 +824,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -841,7 +841,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>29</v>
       </c>
@@ -858,7 +858,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>43075</v>
       </c>
@@ -875,7 +875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>42412</v>
       </c>
@@ -892,7 +892,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>30</v>
       </c>
@@ -909,7 +909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>43105</v>
       </c>
@@ -926,7 +926,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>31</v>
       </c>
@@ -943,7 +943,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>40518</v>
       </c>
@@ -960,7 +960,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>32</v>
       </c>
@@ -977,7 +977,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>33</v>
       </c>
@@ -994,7 +994,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>40487</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>42558</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
@@ -1045,7 +1045,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>41034</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>44632</v>
       </c>
@@ -1096,7 +1096,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>43954</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>36</v>
       </c>
@@ -1130,7 +1130,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>43073</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>43384</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>38</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>40392</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>41498</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -1249,7 +1249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>39876</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>41522</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>41674</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>42</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>42675</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>43</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>43020</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>44</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>45</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>39510</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>46</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>47</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>44291</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>39968</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>48</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>49</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>50</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>51</v>
       </c>
@@ -1589,7 +1589,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>52</v>
       </c>
@@ -1606,7 +1606,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>53</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>39915</v>
       </c>
@@ -1640,7 +1640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>54</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>46</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>39816</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>55</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>56</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>57</v>
       </c>
@@ -1742,7 +1742,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>44176</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>42772</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>58</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>44899</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>39634</v>
       </c>
@@ -1827,7 +1827,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>41853</v>
       </c>
@@ -1844,7 +1844,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>41914</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>41584</v>
       </c>
@@ -1878,7 +1878,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>59</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>41061</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>60</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>44683</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>44654</v>
       </c>
@@ -1963,7 +1963,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>41761</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>61</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>41677</v>
       </c>
@@ -2014,7 +2014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>41334</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>62</v>
       </c>
@@ -2048,7 +2048,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>63</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>64</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>65</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>66</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>67</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>68</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>43962</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>69</v>
       </c>
@@ -2184,7 +2184,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>40059</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
         <v>43835</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
         <v>41764</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>70</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>71</v>
       </c>
@@ -2269,7 +2269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
         <v>44750</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>72</v>
       </c>
@@ -2361,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44539017-217C-4D78-A435-4BE20DCA16A1}">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2902,8 +2902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3747D3F4-8DD7-4813-8D26-0B6B43B43A2C}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Implemented the Sprectrum Allocation for Each Spectrum
</commit_message>
<xml_diff>
--- a/Excel/spectrumRange.xlsx
+++ b/Excel/spectrumRange.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\IIITD\FIRST_SEM\OOPD\Project\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E6F406-1903-46C7-AE9C-3C8BCD9C9C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357F5601-0E89-4773-82F5-FC4B170CF2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spectrumRange" sheetId="1" r:id="rId1"/>
@@ -543,7 +543,7 @@
   <dimension ref="A1:O101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2361,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44539017-217C-4D78-A435-4BE20DCA16A1}">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U16" sqref="U16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2467,6 +2467,10 @@
       <c r="D3" s="1">
         <v>15</v>
       </c>
+      <c r="K3">
+        <f>SUM(K1:K2)</f>
+        <v>40</v>
+      </c>
       <c r="N3" s="1" t="s">
         <v>16</v>
       </c>
@@ -2531,6 +2535,10 @@
       <c r="D5" s="1">
         <v>21</v>
       </c>
+      <c r="P5">
+        <f>SUM(P1:P4)</f>
+        <v>91</v>
+      </c>
       <c r="S5" s="1" t="s">
         <v>7</v>
       </c>
@@ -2554,6 +2562,10 @@
       <c r="D6" s="1">
         <v>20</v>
       </c>
+      <c r="U6">
+        <f>SUM(U1:U5)</f>
+        <v>102</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -2742,6 +2754,14 @@
       <c r="K13" s="1">
         <v>14</v>
       </c>
+      <c r="P13">
+        <f>SUM(P10:P12)</f>
+        <v>46</v>
+      </c>
+      <c r="U13">
+        <f>SUM(U10:U12)</f>
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -2778,6 +2798,10 @@
       </c>
       <c r="D15" s="1">
         <v>22</v>
+      </c>
+      <c r="K15">
+        <f>SUM(K10:K14)</f>
+        <v>107</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -2902,7 +2926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3747D3F4-8DD7-4813-8D26-0B6B43B43A2C}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implemented the revenueGenerated per Spectrum
</commit_message>
<xml_diff>
--- a/Excel/spectrumRange.xlsx
+++ b/Excel/spectrumRange.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\IIITD\FIRST_SEM\OOPD\Project\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357F5601-0E89-4773-82F5-FC4B170CF2E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFCDE99-A4D5-4719-B547-8D25AABA86F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spectrumRange" sheetId="1" r:id="rId1"/>
@@ -2361,8 +2361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44539017-217C-4D78-A435-4BE20DCA16A1}">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3514,7 +3514,7 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4018,6 +4018,10 @@
       <c r="D18" s="1">
         <v>13</v>
       </c>
+      <c r="K18">
+        <f>SUM(K13:K17)</f>
+        <v>116</v>
+      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -4169,8 +4173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3092DA-36D5-4522-BFC9-76788A9DDBC5}">
   <dimension ref="A1:U28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4308,6 +4312,10 @@
       <c r="D4" s="1">
         <v>25</v>
       </c>
+      <c r="K4">
+        <f>SUM(K1:K3)</f>
+        <v>67</v>
+      </c>
       <c r="N4" s="1" t="s">
         <v>7</v>
       </c>
@@ -4609,6 +4617,10 @@
       </c>
       <c r="P14" s="1">
         <v>16</v>
+      </c>
+      <c r="U14">
+        <f>SUM(U9:U13)</f>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>